<commit_message>
fix fast simulation bit array
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/65e5ba34f41e25e0/lab/aespa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="854" documentId="13_ncr:40009_{B2571C16-CD38-4085-A61D-8240FBC2AD0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5AE5467E-1286-4F13-9FFB-4B643C461AC9}"/>
+  <xr:revisionPtr revIDLastSave="856" documentId="13_ncr:40009_{B2571C16-CD38-4085-A61D-8240FBC2AD0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD04D844-19AE-43A6-AA5C-52FB5E5A2502}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-11430" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16320" yWindow="3360" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
@@ -1304,16 +1304,16 @@
   <dimension ref="A1:L106"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I85" sqref="I85"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J89" sqref="J89"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
   <cols>
     <col min="1" max="1" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1351,7 +1351,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A2" s="1">
         <v>44768</v>
       </c>
@@ -1362,10 +1362,10 @@
         <v>10</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E2">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -1389,7 +1389,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A3" s="1">
         <v>44768</v>
       </c>
@@ -1400,11 +1400,10 @@
         <v>10</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D51" si="0">D2</f>
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E3">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1428,7 +1427,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A4" s="1">
         <v>44768</v>
       </c>
@@ -1439,11 +1438,10 @@
         <v>10</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E4">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -1467,7 +1465,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A5" s="1">
         <v>44768</v>
       </c>
@@ -1478,11 +1476,10 @@
         <v>10</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E5">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -1506,7 +1503,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A6" s="1">
         <v>44768</v>
       </c>
@@ -1517,11 +1514,10 @@
         <v>10</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E6">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -1545,7 +1541,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A7" s="1">
         <v>44768</v>
       </c>
@@ -1556,11 +1552,10 @@
         <v>10</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E7">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -1584,7 +1579,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A8" s="1">
         <v>44768</v>
       </c>
@@ -1595,11 +1590,10 @@
         <v>10</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E8">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -1623,7 +1617,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A9" s="1">
         <v>44768</v>
       </c>
@@ -1634,11 +1628,10 @@
         <v>10</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E9">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -1662,7 +1655,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A10" s="1">
         <v>44768</v>
       </c>
@@ -1673,11 +1666,10 @@
         <v>10</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E10">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -1701,7 +1693,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A11" s="1">
         <v>44768</v>
       </c>
@@ -1712,11 +1704,10 @@
         <v>10</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E11">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -1740,7 +1731,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A12" s="1">
         <v>44768</v>
       </c>
@@ -1751,10 +1742,10 @@
         <v>30</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E12">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -1778,7 +1769,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A13" s="1">
         <v>44768</v>
       </c>
@@ -1789,10 +1780,10 @@
         <v>30</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E13">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -1816,7 +1807,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A14" s="1">
         <v>44768</v>
       </c>
@@ -1827,10 +1818,10 @@
         <v>30</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E14">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -1854,7 +1845,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A15" s="1">
         <v>44768</v>
       </c>
@@ -1865,10 +1856,10 @@
         <v>30</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E15">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -1892,7 +1883,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A16" s="1">
         <v>44768</v>
       </c>
@@ -1903,10 +1894,10 @@
         <v>30</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E16">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -1930,7 +1921,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A17" s="1">
         <v>44768</v>
       </c>
@@ -1941,10 +1932,10 @@
         <v>30</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E17">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -1968,7 +1959,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A18" s="1">
         <v>44768</v>
       </c>
@@ -1979,10 +1970,10 @@
         <v>30</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E18">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -2006,7 +1997,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A19" s="1">
         <v>44768</v>
       </c>
@@ -2017,10 +2008,10 @@
         <v>30</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E19">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -2044,7 +2035,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A20" s="1">
         <v>44768</v>
       </c>
@@ -2055,10 +2046,10 @@
         <v>30</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E20">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F20">
         <v>0</v>
@@ -2082,7 +2073,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A21" s="1">
         <v>44768</v>
       </c>
@@ -2093,10 +2084,10 @@
         <v>30</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E21">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F21">
         <v>0</v>
@@ -2120,7 +2111,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A22" s="1">
         <v>44768</v>
       </c>
@@ -2131,10 +2122,10 @@
         <v>70</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E22">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F22">
         <v>0</v>
@@ -2158,7 +2149,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A23" s="1">
         <v>44768</v>
       </c>
@@ -2169,10 +2160,10 @@
         <v>70</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E23">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -2196,7 +2187,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A24" s="1">
         <v>44768</v>
       </c>
@@ -2207,10 +2198,10 @@
         <v>70</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E24">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -2234,7 +2225,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A25" s="1">
         <v>44768</v>
       </c>
@@ -2245,10 +2236,10 @@
         <v>70</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E25">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -2272,7 +2263,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A26" s="1">
         <v>44768</v>
       </c>
@@ -2283,10 +2274,10 @@
         <v>70</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E26">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -2310,7 +2301,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A27" s="1">
         <v>44768</v>
       </c>
@@ -2321,10 +2312,10 @@
         <v>70</v>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E27">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F27">
         <v>0</v>
@@ -2348,7 +2339,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A28" s="1">
         <v>44768</v>
       </c>
@@ -2359,10 +2350,10 @@
         <v>70</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E28">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F28">
         <v>0</v>
@@ -2386,7 +2377,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A29" s="1">
         <v>44768</v>
       </c>
@@ -2397,10 +2388,10 @@
         <v>70</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E29">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -2424,7 +2415,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A30" s="1">
         <v>44768</v>
       </c>
@@ -2435,10 +2426,10 @@
         <v>70</v>
       </c>
       <c r="D30">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E30">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F30">
         <v>0</v>
@@ -2462,7 +2453,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A31" s="1">
         <v>44768</v>
       </c>
@@ -2473,10 +2464,10 @@
         <v>70</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E31">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F31">
         <v>0</v>
@@ -2500,7 +2491,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A32" s="1">
         <v>44768</v>
       </c>
@@ -2511,10 +2502,10 @@
         <v>90</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E32">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F32">
         <v>0</v>
@@ -2538,7 +2529,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A33" s="1">
         <v>44768</v>
       </c>
@@ -2549,10 +2540,10 @@
         <v>90</v>
       </c>
       <c r="D33">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E33">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F33">
         <v>0</v>
@@ -2576,7 +2567,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A34" s="1">
         <v>44768</v>
       </c>
@@ -2587,10 +2578,10 @@
         <v>90</v>
       </c>
       <c r="D34">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E34">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F34">
         <v>0</v>
@@ -2614,7 +2605,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A35" s="1">
         <v>44768</v>
       </c>
@@ -2625,10 +2616,10 @@
         <v>90</v>
       </c>
       <c r="D35">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E35">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F35">
         <v>0</v>
@@ -2652,7 +2643,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A36" s="1">
         <v>44768</v>
       </c>
@@ -2663,10 +2654,10 @@
         <v>90</v>
       </c>
       <c r="D36">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E36">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F36">
         <v>0</v>
@@ -2690,7 +2681,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A37" s="1">
         <v>44768</v>
       </c>
@@ -2701,10 +2692,10 @@
         <v>90</v>
       </c>
       <c r="D37">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E37">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F37">
         <v>0</v>
@@ -2728,7 +2719,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A38" s="1">
         <v>44768</v>
       </c>
@@ -2739,10 +2730,10 @@
         <v>90</v>
       </c>
       <c r="D38">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E38">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F38">
         <v>0</v>
@@ -2766,7 +2757,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A39" s="1">
         <v>44768</v>
       </c>
@@ -2777,10 +2768,10 @@
         <v>90</v>
       </c>
       <c r="D39">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E39">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F39">
         <v>0</v>
@@ -2804,7 +2795,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A40" s="1">
         <v>44768</v>
       </c>
@@ -2815,10 +2806,10 @@
         <v>90</v>
       </c>
       <c r="D40">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E40">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F40">
         <v>0</v>
@@ -2842,7 +2833,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A41" s="1">
         <v>44768</v>
       </c>
@@ -2853,10 +2844,10 @@
         <v>90</v>
       </c>
       <c r="D41">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E41">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F41">
         <v>0</v>
@@ -2880,7 +2871,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A42" s="1">
         <v>44768</v>
       </c>
@@ -2891,10 +2882,10 @@
         <v>20</v>
       </c>
       <c r="D42">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E42">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F42">
         <v>0</v>
@@ -2918,7 +2909,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A43" s="1">
         <v>44768</v>
       </c>
@@ -2929,10 +2920,10 @@
         <v>20</v>
       </c>
       <c r="D43">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E43">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F43">
         <v>0</v>
@@ -2956,7 +2947,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A44" s="1">
         <v>44768</v>
       </c>
@@ -2967,10 +2958,10 @@
         <v>20</v>
       </c>
       <c r="D44">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E44">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F44">
         <v>0</v>
@@ -2994,7 +2985,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A45" s="1">
         <v>44768</v>
       </c>
@@ -3005,10 +2996,10 @@
         <v>20</v>
       </c>
       <c r="D45">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E45">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F45">
         <v>0</v>
@@ -3032,7 +3023,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A46" s="1">
         <v>44768</v>
       </c>
@@ -3043,10 +3034,10 @@
         <v>20</v>
       </c>
       <c r="D46">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E46">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F46">
         <v>0</v>
@@ -3070,7 +3061,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A47" s="1">
         <v>44768</v>
       </c>
@@ -3081,10 +3072,10 @@
         <v>20</v>
       </c>
       <c r="D47">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E47">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F47">
         <v>0</v>
@@ -3108,7 +3099,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A48" s="1">
         <v>44768</v>
       </c>
@@ -3119,10 +3110,10 @@
         <v>20</v>
       </c>
       <c r="D48">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E48">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F48">
         <v>0</v>
@@ -3146,7 +3137,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A49" s="1">
         <v>44768</v>
       </c>
@@ -3157,10 +3148,10 @@
         <v>20</v>
       </c>
       <c r="D49">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E49">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F49">
         <v>0</v>
@@ -3184,7 +3175,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A50" s="1">
         <v>44768</v>
       </c>
@@ -3195,10 +3186,10 @@
         <v>20</v>
       </c>
       <c r="D50">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E50">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F50">
         <v>0</v>
@@ -3222,7 +3213,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A51" s="1">
         <v>44768</v>
       </c>
@@ -3233,10 +3224,10 @@
         <v>20</v>
       </c>
       <c r="D51">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E51">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F51">
         <v>0</v>
@@ -3260,7 +3251,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A52" s="1">
         <v>44768</v>
       </c>
@@ -3271,10 +3262,10 @@
         <v>40</v>
       </c>
       <c r="D52">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E52">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F52">
         <v>0</v>
@@ -3298,7 +3289,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A53" s="1">
         <v>44768</v>
       </c>
@@ -3309,10 +3300,10 @@
         <v>40</v>
       </c>
       <c r="D53">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E53">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F53">
         <v>0</v>
@@ -3336,7 +3327,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A54" s="1">
         <v>44768</v>
       </c>
@@ -3347,10 +3338,10 @@
         <v>40</v>
       </c>
       <c r="D54">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E54">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F54">
         <v>0</v>
@@ -3374,7 +3365,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A55" s="1">
         <v>44768</v>
       </c>
@@ -3385,10 +3376,10 @@
         <v>40</v>
       </c>
       <c r="D55">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E55">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F55">
         <v>0</v>
@@ -3412,7 +3403,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A56" s="1">
         <v>44768</v>
       </c>
@@ -3423,10 +3414,10 @@
         <v>40</v>
       </c>
       <c r="D56">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E56">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F56">
         <v>0</v>
@@ -3450,7 +3441,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A57" s="1">
         <v>44768</v>
       </c>
@@ -3461,10 +3452,10 @@
         <v>40</v>
       </c>
       <c r="D57">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E57">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F57">
         <v>0</v>
@@ -3488,7 +3479,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A58" s="1">
         <v>44768</v>
       </c>
@@ -3499,10 +3490,10 @@
         <v>40</v>
       </c>
       <c r="D58">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E58">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F58">
         <v>0</v>
@@ -3526,7 +3517,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A59" s="1">
         <v>44768</v>
       </c>
@@ -3537,10 +3528,10 @@
         <v>40</v>
       </c>
       <c r="D59">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E59">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F59">
         <v>0</v>
@@ -3564,7 +3555,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A60" s="1">
         <v>44768</v>
       </c>
@@ -3575,10 +3566,10 @@
         <v>40</v>
       </c>
       <c r="D60">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E60">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F60">
         <v>0</v>
@@ -3602,7 +3593,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A61" s="1">
         <v>44768</v>
       </c>
@@ -3613,10 +3604,10 @@
         <v>40</v>
       </c>
       <c r="D61">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E61">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F61">
         <v>0</v>
@@ -3640,7 +3631,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A62" s="1">
         <v>44768</v>
       </c>
@@ -3651,10 +3642,10 @@
         <v>60</v>
       </c>
       <c r="D62">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E62">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F62">
         <v>0</v>
@@ -3678,7 +3669,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A63" s="1">
         <v>44768</v>
       </c>
@@ -3689,10 +3680,10 @@
         <v>60</v>
       </c>
       <c r="D63">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E63">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F63">
         <v>0</v>
@@ -3716,7 +3707,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A64" s="1">
         <v>44768</v>
       </c>
@@ -3727,10 +3718,10 @@
         <v>60</v>
       </c>
       <c r="D64">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E64">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F64">
         <v>0</v>
@@ -3754,7 +3745,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A65" s="1">
         <v>44768</v>
       </c>
@@ -3765,10 +3756,10 @@
         <v>60</v>
       </c>
       <c r="D65">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E65">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F65">
         <v>0</v>
@@ -3792,7 +3783,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A66" s="1">
         <v>44768</v>
       </c>
@@ -3803,10 +3794,10 @@
         <v>60</v>
       </c>
       <c r="D66">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E66">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F66">
         <v>0</v>
@@ -3830,7 +3821,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A67" s="1">
         <v>44768</v>
       </c>
@@ -3841,10 +3832,10 @@
         <v>60</v>
       </c>
       <c r="D67">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E67">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F67">
         <v>0</v>
@@ -3868,7 +3859,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A68" s="1">
         <v>44768</v>
       </c>
@@ -3879,10 +3870,10 @@
         <v>60</v>
       </c>
       <c r="D68">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E68">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F68">
         <v>0</v>
@@ -3906,7 +3897,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A69" s="1">
         <v>44768</v>
       </c>
@@ -3917,10 +3908,10 @@
         <v>60</v>
       </c>
       <c r="D69">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E69">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F69">
         <v>0</v>
@@ -3944,7 +3935,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A70" s="1">
         <v>44768</v>
       </c>
@@ -3955,10 +3946,10 @@
         <v>60</v>
       </c>
       <c r="D70">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E70">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F70">
         <v>0</v>
@@ -3982,7 +3973,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A71" s="1">
         <v>44768</v>
       </c>
@@ -3993,10 +3984,10 @@
         <v>60</v>
       </c>
       <c r="D71">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E71">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F71">
         <v>0</v>
@@ -4020,7 +4011,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A72" s="1">
         <v>44768</v>
       </c>
@@ -4031,10 +4022,10 @@
         <v>80</v>
       </c>
       <c r="D72">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E72">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F72">
         <v>0</v>
@@ -4058,7 +4049,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A73" s="1">
         <v>44768</v>
       </c>
@@ -4069,10 +4060,10 @@
         <v>80</v>
       </c>
       <c r="D73">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E73">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F73">
         <v>0</v>
@@ -4096,7 +4087,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A74" s="1">
         <v>44768</v>
       </c>
@@ -4107,10 +4098,10 @@
         <v>80</v>
       </c>
       <c r="D74">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E74">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F74">
         <v>0</v>
@@ -4134,7 +4125,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A75" s="1">
         <v>44768</v>
       </c>
@@ -4145,10 +4136,10 @@
         <v>80</v>
       </c>
       <c r="D75">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E75">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F75">
         <v>0</v>
@@ -4172,7 +4163,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A76" s="1">
         <v>44768</v>
       </c>
@@ -4183,10 +4174,10 @@
         <v>80</v>
       </c>
       <c r="D76">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E76">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F76">
         <v>0</v>
@@ -4210,7 +4201,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A77" s="1">
         <v>44768</v>
       </c>
@@ -4221,10 +4212,10 @@
         <v>80</v>
       </c>
       <c r="D77">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E77">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F77">
         <v>0</v>
@@ -4248,7 +4239,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A78" s="1">
         <v>44768</v>
       </c>
@@ -4259,10 +4250,10 @@
         <v>80</v>
       </c>
       <c r="D78">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E78">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F78">
         <v>0</v>
@@ -4286,7 +4277,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A79" s="1">
         <v>44768</v>
       </c>
@@ -4297,10 +4288,10 @@
         <v>80</v>
       </c>
       <c r="D79">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E79">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F79">
         <v>0</v>
@@ -4324,7 +4315,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A80" s="1">
         <v>44768</v>
       </c>
@@ -4335,10 +4326,10 @@
         <v>80</v>
       </c>
       <c r="D80">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E80">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F80">
         <v>0</v>
@@ -4362,7 +4353,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A81" s="1">
         <v>44768</v>
       </c>
@@ -4373,10 +4364,10 @@
         <v>80</v>
       </c>
       <c r="D81">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="E81">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F81">
         <v>0</v>
@@ -4400,7 +4391,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A82" s="1">
         <v>44768</v>
       </c>
@@ -4414,7 +4405,7 @@
         <v>601</v>
       </c>
       <c r="E82">
-        <f t="shared" ref="E82:E91" si="1">D82+9</f>
+        <f t="shared" ref="E82:E91" si="0">D82+9</f>
         <v>610</v>
       </c>
       <c r="F82">
@@ -4439,7 +4430,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A83" s="1">
         <v>44768</v>
       </c>
@@ -4454,7 +4445,7 @@
         <v>611</v>
       </c>
       <c r="E83">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>620</v>
       </c>
       <c r="F83">
@@ -4479,7 +4470,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A84" s="1">
         <v>44768</v>
       </c>
@@ -4490,11 +4481,11 @@
         <v>50</v>
       </c>
       <c r="D84">
-        <f t="shared" ref="D84:D101" si="2">D83+10</f>
+        <f t="shared" ref="D84:D101" si="1">D83+10</f>
         <v>621</v>
       </c>
       <c r="E84">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>630</v>
       </c>
       <c r="F84">
@@ -4519,7 +4510,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A85" s="1">
         <v>44768</v>
       </c>
@@ -4530,11 +4521,11 @@
         <v>50</v>
       </c>
       <c r="D85">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>631</v>
       </c>
       <c r="E85">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>640</v>
       </c>
       <c r="F85">
@@ -4559,7 +4550,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A86" s="1">
         <v>44768</v>
       </c>
@@ -4570,11 +4561,11 @@
         <v>50</v>
       </c>
       <c r="D86">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>641</v>
       </c>
       <c r="E86">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>650</v>
       </c>
       <c r="F86">
@@ -4599,7 +4590,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A87" s="1">
         <v>44768</v>
       </c>
@@ -4610,11 +4601,11 @@
         <v>50</v>
       </c>
       <c r="D87">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>651</v>
       </c>
       <c r="E87">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>660</v>
       </c>
       <c r="F87">
@@ -4639,7 +4630,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A88" s="1">
         <v>44768</v>
       </c>
@@ -4650,11 +4641,11 @@
         <v>50</v>
       </c>
       <c r="D88">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>661</v>
       </c>
       <c r="E88">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>670</v>
       </c>
       <c r="F88">
@@ -4679,7 +4670,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A89" s="1">
         <v>44768</v>
       </c>
@@ -4690,11 +4681,11 @@
         <v>50</v>
       </c>
       <c r="D89">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>671</v>
       </c>
       <c r="E89">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>680</v>
       </c>
       <c r="F89">
@@ -4719,7 +4710,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A90" s="1">
         <v>44768</v>
       </c>
@@ -4730,11 +4721,11 @@
         <v>50</v>
       </c>
       <c r="D90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>681</v>
       </c>
       <c r="E90">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>690</v>
       </c>
       <c r="F90">
@@ -4759,7 +4750,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A91" s="1">
         <v>44768</v>
       </c>
@@ -4770,11 +4761,11 @@
         <v>50</v>
       </c>
       <c r="D91">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>691</v>
       </c>
       <c r="E91">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>700</v>
       </c>
       <c r="F91">
@@ -4799,7 +4790,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A92" s="1">
         <v>44768</v>
       </c>
@@ -4810,11 +4801,11 @@
         <v>50</v>
       </c>
       <c r="D92">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>701</v>
       </c>
       <c r="E92">
-        <f t="shared" ref="E92:E101" si="3">D92+9</f>
+        <f t="shared" ref="E92:E101" si="2">D92+9</f>
         <v>710</v>
       </c>
       <c r="F92">
@@ -4839,7 +4830,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A93" s="1">
         <v>44768</v>
       </c>
@@ -4850,11 +4841,11 @@
         <v>50</v>
       </c>
       <c r="D93">
+        <f t="shared" si="1"/>
+        <v>711</v>
+      </c>
+      <c r="E93">
         <f t="shared" si="2"/>
-        <v>711</v>
-      </c>
-      <c r="E93">
-        <f t="shared" si="3"/>
         <v>720</v>
       </c>
       <c r="F93">
@@ -4879,7 +4870,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A94" s="1">
         <v>44768</v>
       </c>
@@ -4890,11 +4881,11 @@
         <v>50</v>
       </c>
       <c r="D94">
+        <f t="shared" si="1"/>
+        <v>721</v>
+      </c>
+      <c r="E94">
         <f t="shared" si="2"/>
-        <v>721</v>
-      </c>
-      <c r="E94">
-        <f t="shared" si="3"/>
         <v>730</v>
       </c>
       <c r="F94">
@@ -4919,7 +4910,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A95" s="1">
         <v>44768</v>
       </c>
@@ -4930,11 +4921,11 @@
         <v>50</v>
       </c>
       <c r="D95">
+        <f t="shared" si="1"/>
+        <v>731</v>
+      </c>
+      <c r="E95">
         <f t="shared" si="2"/>
-        <v>731</v>
-      </c>
-      <c r="E95">
-        <f t="shared" si="3"/>
         <v>740</v>
       </c>
       <c r="F95">
@@ -4959,7 +4950,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A96" s="1">
         <v>44768</v>
       </c>
@@ -4970,11 +4961,11 @@
         <v>50</v>
       </c>
       <c r="D96">
+        <f t="shared" si="1"/>
+        <v>741</v>
+      </c>
+      <c r="E96">
         <f t="shared" si="2"/>
-        <v>741</v>
-      </c>
-      <c r="E96">
-        <f t="shared" si="3"/>
         <v>750</v>
       </c>
       <c r="F96">
@@ -4999,7 +4990,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A97" s="1">
         <v>44768</v>
       </c>
@@ -5010,11 +5001,11 @@
         <v>50</v>
       </c>
       <c r="D97">
+        <f t="shared" si="1"/>
+        <v>751</v>
+      </c>
+      <c r="E97">
         <f t="shared" si="2"/>
-        <v>751</v>
-      </c>
-      <c r="E97">
-        <f t="shared" si="3"/>
         <v>760</v>
       </c>
       <c r="F97">
@@ -5039,7 +5030,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A98" s="1">
         <v>44768</v>
       </c>
@@ -5050,11 +5041,11 @@
         <v>50</v>
       </c>
       <c r="D98">
+        <f t="shared" si="1"/>
+        <v>761</v>
+      </c>
+      <c r="E98">
         <f t="shared" si="2"/>
-        <v>761</v>
-      </c>
-      <c r="E98">
-        <f t="shared" si="3"/>
         <v>770</v>
       </c>
       <c r="F98">
@@ -5079,7 +5070,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A99" s="1">
         <v>44768</v>
       </c>
@@ -5090,11 +5081,11 @@
         <v>50</v>
       </c>
       <c r="D99">
+        <f t="shared" si="1"/>
+        <v>771</v>
+      </c>
+      <c r="E99">
         <f t="shared" si="2"/>
-        <v>771</v>
-      </c>
-      <c r="E99">
-        <f t="shared" si="3"/>
         <v>780</v>
       </c>
       <c r="F99">
@@ -5119,7 +5110,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A100" s="1">
         <v>44768</v>
       </c>
@@ -5130,11 +5121,11 @@
         <v>50</v>
       </c>
       <c r="D100">
+        <f t="shared" si="1"/>
+        <v>781</v>
+      </c>
+      <c r="E100">
         <f t="shared" si="2"/>
-        <v>781</v>
-      </c>
-      <c r="E100">
-        <f t="shared" si="3"/>
         <v>790</v>
       </c>
       <c r="F100">
@@ -5159,7 +5150,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A101" s="1">
         <v>44768</v>
       </c>
@@ -5170,11 +5161,11 @@
         <v>50</v>
       </c>
       <c r="D101">
+        <f t="shared" si="1"/>
+        <v>791</v>
+      </c>
+      <c r="E101">
         <f t="shared" si="2"/>
-        <v>791</v>
-      </c>
-      <c r="E101">
-        <f t="shared" si="3"/>
         <v>800</v>
       </c>
       <c r="F101">
@@ -5199,19 +5190,19 @@
         <v>14</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A102" s="1"/>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A103" s="1"/>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A104" s="1"/>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A105" s="1"/>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.6">
       <c r="A106" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix the Error Reporting
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/65e5ba34f41e25e0/lab/aespa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="978" documentId="13_ncr:40009_{B2571C16-CD38-4085-A61D-8240FBC2AD0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A4FBD03-9FC6-4493-A177-3C52C14C7FFC}"/>
+  <xr:revisionPtr revIDLastSave="982" documentId="13_ncr:40009_{B2571C16-CD38-4085-A61D-8240FBC2AD0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{719B4396-91A7-426A-9428-7C67E2D8B3B0}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1057,8 +1057,8 @@
   <dimension ref="A1:K226"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A206" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H219" sqref="H219"/>
+      <pane ySplit="1" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M110" sqref="M110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1110,10 +1110,10 @@
         <v>MM010010</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D2">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E2">
         <v>10</v>
@@ -1143,10 +1143,10 @@
         <v>MM020010</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D3">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E3">
         <v>20</v>
@@ -1176,10 +1176,10 @@
         <v>MM030010</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D4">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E4">
         <v>30</v>
@@ -1209,10 +1209,10 @@
         <v>MM040010</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D5">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E5">
         <v>40</v>
@@ -1242,10 +1242,10 @@
         <v>MM050010</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D6">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E6">
         <v>50</v>
@@ -1275,10 +1275,10 @@
         <v>MM060010</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D7">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E7">
         <v>60</v>
@@ -1308,10 +1308,10 @@
         <v>MM070010</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D8">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E8">
         <v>70</v>
@@ -1341,10 +1341,10 @@
         <v>MM080010</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D9">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E9">
         <v>80</v>
@@ -1374,10 +1374,10 @@
         <v>MM090010</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D10">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E10">
         <v>90</v>
@@ -1407,10 +1407,10 @@
         <v>MM100010</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D11">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E11">
         <v>100</v>
@@ -1440,10 +1440,10 @@
         <v>MM010020</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D12">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E12">
         <v>10</v>
@@ -1474,10 +1474,10 @@
         <v>MM020020</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D13">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E13">
         <v>20</v>
@@ -1508,10 +1508,10 @@
         <v>MM030020</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D14">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E14">
         <v>30</v>
@@ -1542,10 +1542,10 @@
         <v>MM040020</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D15">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E15">
         <v>40</v>
@@ -1576,10 +1576,10 @@
         <v>MM050020</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D16">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E16">
         <v>50</v>
@@ -1610,10 +1610,10 @@
         <v>MM060020</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D17">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E17">
         <v>60</v>
@@ -1644,10 +1644,10 @@
         <v>MM070020</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D18">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E18">
         <v>70</v>
@@ -1678,10 +1678,10 @@
         <v>MM080020</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D19">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E19">
         <v>80</v>
@@ -1712,10 +1712,10 @@
         <v>MM090020</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D20">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E20">
         <v>90</v>
@@ -1746,10 +1746,10 @@
         <v>MM100020</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D21">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E21">
         <v>100</v>
@@ -1780,10 +1780,10 @@
         <v>MM010030</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D22">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E22">
         <v>10</v>
@@ -1814,10 +1814,10 @@
         <v>MM020030</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D23">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E23">
         <v>20</v>
@@ -1848,10 +1848,10 @@
         <v>MM030030</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D24">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E24">
         <v>30</v>
@@ -1882,10 +1882,10 @@
         <v>MM040030</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D25">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E25">
         <v>40</v>
@@ -1916,10 +1916,10 @@
         <v>MM050030</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D26">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E26">
         <v>50</v>
@@ -1950,10 +1950,10 @@
         <v>MM060030</v>
       </c>
       <c r="C27">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D27">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E27">
         <v>60</v>
@@ -1984,10 +1984,10 @@
         <v>MM070030</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D28">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E28">
         <v>70</v>
@@ -2018,10 +2018,10 @@
         <v>MM080030</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D29">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E29">
         <v>80</v>
@@ -2052,10 +2052,10 @@
         <v>MM090030</v>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D30">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E30">
         <v>90</v>
@@ -2086,10 +2086,10 @@
         <v>MM100030</v>
       </c>
       <c r="C31">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D31">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E31">
         <v>100</v>
@@ -2120,10 +2120,10 @@
         <v>MM010040</v>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D32">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E32">
         <v>10</v>
@@ -2154,10 +2154,10 @@
         <v>MM020040</v>
       </c>
       <c r="C33">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D33">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E33">
         <v>20</v>
@@ -2188,10 +2188,10 @@
         <v>MM030040</v>
       </c>
       <c r="C34">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D34">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E34">
         <v>30</v>
@@ -2222,10 +2222,10 @@
         <v>MM040040</v>
       </c>
       <c r="C35">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D35">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E35">
         <v>40</v>
@@ -2256,10 +2256,10 @@
         <v>MM050040</v>
       </c>
       <c r="C36">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D36">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E36">
         <v>50</v>
@@ -2290,10 +2290,10 @@
         <v>MM060040</v>
       </c>
       <c r="C37">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D37">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E37">
         <v>60</v>
@@ -2324,10 +2324,10 @@
         <v>MM070040</v>
       </c>
       <c r="C38">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D38">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E38">
         <v>70</v>
@@ -2358,10 +2358,10 @@
         <v>MM080040</v>
       </c>
       <c r="C39">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D39">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E39">
         <v>80</v>
@@ -2392,10 +2392,10 @@
         <v>MM090040</v>
       </c>
       <c r="C40">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D40">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E40">
         <v>90</v>
@@ -2426,10 +2426,10 @@
         <v>MM100040</v>
       </c>
       <c r="C41">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D41">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E41">
         <v>100</v>
@@ -2460,10 +2460,10 @@
         <v>MM010050</v>
       </c>
       <c r="C42">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D42">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E42">
         <v>10</v>
@@ -2494,10 +2494,10 @@
         <v>MM020050</v>
       </c>
       <c r="C43">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D43">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E43">
         <v>20</v>
@@ -2528,10 +2528,10 @@
         <v>MM030050</v>
       </c>
       <c r="C44">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D44">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E44">
         <v>30</v>
@@ -2562,10 +2562,10 @@
         <v>MM040050</v>
       </c>
       <c r="C45">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D45">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E45">
         <v>40</v>
@@ -2596,10 +2596,10 @@
         <v>MM050050</v>
       </c>
       <c r="C46">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D46">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E46">
         <v>50</v>
@@ -2630,10 +2630,10 @@
         <v>MM060050</v>
       </c>
       <c r="C47">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D47">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E47">
         <v>60</v>
@@ -2664,10 +2664,10 @@
         <v>MM070050</v>
       </c>
       <c r="C48">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D48">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E48">
         <v>70</v>
@@ -2698,10 +2698,10 @@
         <v>MM080050</v>
       </c>
       <c r="C49">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D49">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E49">
         <v>80</v>
@@ -2732,10 +2732,10 @@
         <v>MM090050</v>
       </c>
       <c r="C50">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D50">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E50">
         <v>90</v>
@@ -2766,10 +2766,10 @@
         <v>MM100050</v>
       </c>
       <c r="C51">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D51">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E51">
         <v>100</v>
@@ -2800,10 +2800,10 @@
         <v>MM010060</v>
       </c>
       <c r="C52">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D52">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E52">
         <v>10</v>
@@ -2834,10 +2834,10 @@
         <v>MM020060</v>
       </c>
       <c r="C53">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D53">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E53">
         <v>20</v>
@@ -2868,10 +2868,10 @@
         <v>MM030060</v>
       </c>
       <c r="C54">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D54">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E54">
         <v>30</v>
@@ -2902,10 +2902,10 @@
         <v>MM040060</v>
       </c>
       <c r="C55">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D55">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E55">
         <v>40</v>
@@ -2936,10 +2936,10 @@
         <v>MM050060</v>
       </c>
       <c r="C56">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D56">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E56">
         <v>50</v>
@@ -2970,10 +2970,10 @@
         <v>MM060060</v>
       </c>
       <c r="C57">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D57">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E57">
         <v>60</v>
@@ -3004,10 +3004,10 @@
         <v>MM070060</v>
       </c>
       <c r="C58">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D58">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E58">
         <v>70</v>
@@ -3038,10 +3038,10 @@
         <v>MM080060</v>
       </c>
       <c r="C59">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D59">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E59">
         <v>80</v>
@@ -3072,10 +3072,10 @@
         <v>MM090060</v>
       </c>
       <c r="C60">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D60">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E60">
         <v>90</v>
@@ -3106,10 +3106,10 @@
         <v>MM100060</v>
       </c>
       <c r="C61">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D61">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E61">
         <v>100</v>
@@ -3140,10 +3140,10 @@
         <v>MM010070</v>
       </c>
       <c r="C62">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D62">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E62">
         <v>10</v>
@@ -3174,10 +3174,10 @@
         <v>MM020070</v>
       </c>
       <c r="C63">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D63">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E63">
         <v>20</v>
@@ -3208,10 +3208,10 @@
         <v>MM030070</v>
       </c>
       <c r="C64">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D64">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E64">
         <v>30</v>
@@ -3242,10 +3242,10 @@
         <v>MM040070</v>
       </c>
       <c r="C65">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D65">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E65">
         <v>40</v>
@@ -3276,10 +3276,10 @@
         <v>MM050070</v>
       </c>
       <c r="C66">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D66">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E66">
         <v>50</v>
@@ -3310,10 +3310,10 @@
         <v>MM060070</v>
       </c>
       <c r="C67">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D67">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E67">
         <v>60</v>
@@ -3344,10 +3344,10 @@
         <v>MM070070</v>
       </c>
       <c r="C68">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D68">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E68">
         <v>70</v>
@@ -3378,10 +3378,10 @@
         <v>MM080070</v>
       </c>
       <c r="C69">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D69">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E69">
         <v>80</v>
@@ -3412,10 +3412,10 @@
         <v>MM090070</v>
       </c>
       <c r="C70">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D70">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E70">
         <v>90</v>
@@ -3446,10 +3446,10 @@
         <v>MM100070</v>
       </c>
       <c r="C71">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D71">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E71">
         <v>100</v>
@@ -3480,10 +3480,10 @@
         <v>MM010080</v>
       </c>
       <c r="C72">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D72">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E72">
         <v>10</v>
@@ -3514,10 +3514,10 @@
         <v>MM020080</v>
       </c>
       <c r="C73">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D73">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E73">
         <v>20</v>
@@ -3548,10 +3548,10 @@
         <v>MM030080</v>
       </c>
       <c r="C74">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D74">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E74">
         <v>30</v>
@@ -3582,10 +3582,10 @@
         <v>MM040080</v>
       </c>
       <c r="C75">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D75">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E75">
         <v>40</v>
@@ -3616,10 +3616,10 @@
         <v>MM050080</v>
       </c>
       <c r="C76">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D76">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E76">
         <v>50</v>
@@ -3650,10 +3650,10 @@
         <v>MM060080</v>
       </c>
       <c r="C77">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D77">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E77">
         <v>60</v>
@@ -3684,10 +3684,10 @@
         <v>MM070080</v>
       </c>
       <c r="C78">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D78">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E78">
         <v>70</v>
@@ -3718,10 +3718,10 @@
         <v>MM080080</v>
       </c>
       <c r="C79">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D79">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E79">
         <v>80</v>
@@ -3752,10 +3752,10 @@
         <v>MM090080</v>
       </c>
       <c r="C80">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D80">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E80">
         <v>90</v>
@@ -3786,10 +3786,10 @@
         <v>MM100080</v>
       </c>
       <c r="C81">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D81">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E81">
         <v>100</v>
@@ -3820,10 +3820,10 @@
         <v>MM010090</v>
       </c>
       <c r="C82">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D82">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E82">
         <v>10</v>
@@ -3854,10 +3854,10 @@
         <v>MM020090</v>
       </c>
       <c r="C83">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D83">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E83">
         <v>20</v>
@@ -3888,10 +3888,10 @@
         <v>MM030090</v>
       </c>
       <c r="C84">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D84">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E84">
         <v>30</v>
@@ -3922,10 +3922,10 @@
         <v>MM040090</v>
       </c>
       <c r="C85">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D85">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E85">
         <v>40</v>
@@ -3956,10 +3956,10 @@
         <v>MM050090</v>
       </c>
       <c r="C86">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D86">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E86">
         <v>50</v>
@@ -3990,10 +3990,10 @@
         <v>MM060090</v>
       </c>
       <c r="C87">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D87">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E87">
         <v>60</v>
@@ -4024,10 +4024,10 @@
         <v>MM070090</v>
       </c>
       <c r="C88">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D88">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E88">
         <v>70</v>
@@ -4058,10 +4058,10 @@
         <v>MM080090</v>
       </c>
       <c r="C89">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D89">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E89">
         <v>80</v>
@@ -4092,10 +4092,10 @@
         <v>MM090090</v>
       </c>
       <c r="C90">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D90">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E90">
         <v>90</v>
@@ -4126,10 +4126,10 @@
         <v>MM100090</v>
       </c>
       <c r="C91">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D91">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E91">
         <v>100</v>
@@ -4160,10 +4160,10 @@
         <v>MM010100</v>
       </c>
       <c r="C92">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D92">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E92">
         <v>10</v>
@@ -4194,10 +4194,10 @@
         <v>MM020100</v>
       </c>
       <c r="C93">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D93">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E93">
         <v>20</v>
@@ -4228,10 +4228,10 @@
         <v>MM030100</v>
       </c>
       <c r="C94">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D94">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E94">
         <v>30</v>
@@ -4262,10 +4262,10 @@
         <v>MM040100</v>
       </c>
       <c r="C95">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D95">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E95">
         <v>40</v>
@@ -4296,10 +4296,10 @@
         <v>MM050100</v>
       </c>
       <c r="C96">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D96">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E96">
         <v>50</v>
@@ -4330,10 +4330,10 @@
         <v>MM060100</v>
       </c>
       <c r="C97">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D97">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E97">
         <v>60</v>
@@ -4364,10 +4364,10 @@
         <v>MM070100</v>
       </c>
       <c r="C98">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D98">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E98">
         <v>70</v>
@@ -4398,10 +4398,10 @@
         <v>MM080100</v>
       </c>
       <c r="C99">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D99">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E99">
         <v>80</v>
@@ -4432,10 +4432,10 @@
         <v>MM090100</v>
       </c>
       <c r="C100">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D100">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E100">
         <v>90</v>
@@ -4466,10 +4466,10 @@
         <v>MM100100</v>
       </c>
       <c r="C101">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D101">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E101">
         <v>100</v>
@@ -4503,10 +4503,10 @@
         <v>MM010010</v>
       </c>
       <c r="C102">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D102">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E102">
         <v>10</v>
@@ -4536,10 +4536,10 @@
         <v>MM020010</v>
       </c>
       <c r="C103">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D103">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E103">
         <v>20</v>
@@ -4569,10 +4569,10 @@
         <v>MM030010</v>
       </c>
       <c r="C104">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D104">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E104">
         <v>30</v>
@@ -4602,10 +4602,10 @@
         <v>MM040010</v>
       </c>
       <c r="C105">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D105">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E105">
         <v>40</v>
@@ -4635,10 +4635,10 @@
         <v>MM050010</v>
       </c>
       <c r="C106">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D106">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E106">
         <v>50</v>
@@ -4668,10 +4668,10 @@
         <v>MM060010</v>
       </c>
       <c r="C107">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D107">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E107">
         <v>60</v>
@@ -4701,10 +4701,10 @@
         <v>MM070010</v>
       </c>
       <c r="C108">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D108">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E108">
         <v>70</v>
@@ -4734,10 +4734,10 @@
         <v>MM080010</v>
       </c>
       <c r="C109">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D109">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E109">
         <v>80</v>
@@ -4767,10 +4767,10 @@
         <v>MM090010</v>
       </c>
       <c r="C110">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D110">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E110">
         <v>90</v>
@@ -4800,10 +4800,10 @@
         <v>MM100010</v>
       </c>
       <c r="C111">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D111">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E111">
         <v>100</v>
@@ -4833,10 +4833,10 @@
         <v>MM010020</v>
       </c>
       <c r="C112">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D112">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E112">
         <v>10</v>
@@ -4867,10 +4867,10 @@
         <v>MM020020</v>
       </c>
       <c r="C113">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D113">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E113">
         <v>20</v>
@@ -4901,10 +4901,10 @@
         <v>MM030020</v>
       </c>
       <c r="C114">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D114">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E114">
         <v>30</v>
@@ -4935,10 +4935,10 @@
         <v>MM040020</v>
       </c>
       <c r="C115">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D115">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E115">
         <v>40</v>
@@ -4969,10 +4969,10 @@
         <v>MM050020</v>
       </c>
       <c r="C116">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D116">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E116">
         <v>50</v>
@@ -5003,10 +5003,10 @@
         <v>MM060020</v>
       </c>
       <c r="C117">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D117">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E117">
         <v>60</v>
@@ -5037,10 +5037,10 @@
         <v>MM070020</v>
       </c>
       <c r="C118">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D118">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E118">
         <v>70</v>
@@ -5071,10 +5071,10 @@
         <v>MM080020</v>
       </c>
       <c r="C119">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D119">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E119">
         <v>80</v>
@@ -5105,10 +5105,10 @@
         <v>MM090020</v>
       </c>
       <c r="C120">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D120">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E120">
         <v>90</v>
@@ -5139,10 +5139,10 @@
         <v>MM100020</v>
       </c>
       <c r="C121">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D121">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E121">
         <v>100</v>
@@ -5173,10 +5173,10 @@
         <v>MM010030</v>
       </c>
       <c r="C122">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D122">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E122">
         <v>10</v>
@@ -5207,10 +5207,10 @@
         <v>MM020030</v>
       </c>
       <c r="C123">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D123">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E123">
         <v>20</v>
@@ -5241,10 +5241,10 @@
         <v>MM030030</v>
       </c>
       <c r="C124">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D124">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E124">
         <v>30</v>
@@ -5275,10 +5275,10 @@
         <v>MM040030</v>
       </c>
       <c r="C125">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D125">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E125">
         <v>40</v>
@@ -5309,10 +5309,10 @@
         <v>MM050030</v>
       </c>
       <c r="C126">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D126">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E126">
         <v>50</v>
@@ -5343,10 +5343,10 @@
         <v>MM060030</v>
       </c>
       <c r="C127">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D127">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E127">
         <v>60</v>
@@ -5377,10 +5377,10 @@
         <v>MM070030</v>
       </c>
       <c r="C128">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D128">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E128">
         <v>70</v>
@@ -5411,10 +5411,10 @@
         <v>MM080030</v>
       </c>
       <c r="C129">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D129">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E129">
         <v>80</v>
@@ -5445,10 +5445,10 @@
         <v>MM090030</v>
       </c>
       <c r="C130">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D130">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E130">
         <v>90</v>
@@ -5479,10 +5479,10 @@
         <v>MM100030</v>
       </c>
       <c r="C131">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D131">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E131">
         <v>100</v>
@@ -5513,10 +5513,10 @@
         <v>MM010040</v>
       </c>
       <c r="C132">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D132">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E132">
         <v>10</v>
@@ -5547,10 +5547,10 @@
         <v>MM020040</v>
       </c>
       <c r="C133">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D133">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E133">
         <v>20</v>
@@ -5581,10 +5581,10 @@
         <v>MM030040</v>
       </c>
       <c r="C134">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D134">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E134">
         <v>30</v>
@@ -5615,10 +5615,10 @@
         <v>MM040040</v>
       </c>
       <c r="C135">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D135">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E135">
         <v>40</v>
@@ -5649,10 +5649,10 @@
         <v>MM050040</v>
       </c>
       <c r="C136">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D136">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E136">
         <v>50</v>
@@ -5683,10 +5683,10 @@
         <v>MM060040</v>
       </c>
       <c r="C137">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D137">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E137">
         <v>60</v>
@@ -5717,10 +5717,10 @@
         <v>MM070040</v>
       </c>
       <c r="C138">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D138">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E138">
         <v>70</v>
@@ -5751,10 +5751,10 @@
         <v>MM080040</v>
       </c>
       <c r="C139">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D139">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E139">
         <v>80</v>
@@ -5785,10 +5785,10 @@
         <v>MM090040</v>
       </c>
       <c r="C140">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D140">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E140">
         <v>90</v>
@@ -5819,10 +5819,10 @@
         <v>MM100040</v>
       </c>
       <c r="C141">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D141">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E141">
         <v>100</v>
@@ -5853,10 +5853,10 @@
         <v>MM010050</v>
       </c>
       <c r="C142">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D142">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E142">
         <v>10</v>
@@ -5887,10 +5887,10 @@
         <v>MM020050</v>
       </c>
       <c r="C143">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D143">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E143">
         <v>20</v>
@@ -5921,10 +5921,10 @@
         <v>MM030050</v>
       </c>
       <c r="C144">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D144">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E144">
         <v>30</v>
@@ -5955,10 +5955,10 @@
         <v>MM040050</v>
       </c>
       <c r="C145">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D145">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E145">
         <v>40</v>
@@ -5989,10 +5989,10 @@
         <v>MM050050</v>
       </c>
       <c r="C146">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D146">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E146">
         <v>50</v>
@@ -6023,10 +6023,10 @@
         <v>MM060050</v>
       </c>
       <c r="C147">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D147">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E147">
         <v>60</v>
@@ -6057,10 +6057,10 @@
         <v>MM070050</v>
       </c>
       <c r="C148">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D148">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E148">
         <v>70</v>
@@ -6091,10 +6091,10 @@
         <v>MM080050</v>
       </c>
       <c r="C149">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D149">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E149">
         <v>80</v>
@@ -6125,10 +6125,10 @@
         <v>MM090050</v>
       </c>
       <c r="C150">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D150">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E150">
         <v>90</v>
@@ -6159,10 +6159,10 @@
         <v>MM100050</v>
       </c>
       <c r="C151">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D151">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E151">
         <v>100</v>
@@ -6193,10 +6193,10 @@
         <v>MM010060</v>
       </c>
       <c r="C152">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D152">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E152">
         <v>10</v>
@@ -6227,10 +6227,10 @@
         <v>MM020060</v>
       </c>
       <c r="C153">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D153">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E153">
         <v>20</v>
@@ -6261,10 +6261,10 @@
         <v>MM030060</v>
       </c>
       <c r="C154">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D154">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E154">
         <v>30</v>
@@ -6295,10 +6295,10 @@
         <v>MM040060</v>
       </c>
       <c r="C155">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D155">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E155">
         <v>40</v>
@@ -6329,10 +6329,10 @@
         <v>MM050060</v>
       </c>
       <c r="C156">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D156">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E156">
         <v>50</v>
@@ -6363,10 +6363,10 @@
         <v>MM060060</v>
       </c>
       <c r="C157">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D157">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E157">
         <v>60</v>
@@ -6397,10 +6397,10 @@
         <v>MM070060</v>
       </c>
       <c r="C158">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D158">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E158">
         <v>70</v>
@@ -6431,10 +6431,10 @@
         <v>MM080060</v>
       </c>
       <c r="C159">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D159">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E159">
         <v>80</v>
@@ -6465,10 +6465,10 @@
         <v>MM090060</v>
       </c>
       <c r="C160">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D160">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E160">
         <v>90</v>
@@ -6499,10 +6499,10 @@
         <v>MM100060</v>
       </c>
       <c r="C161">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D161">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E161">
         <v>100</v>
@@ -6533,10 +6533,10 @@
         <v>MM010070</v>
       </c>
       <c r="C162">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D162">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E162">
         <v>10</v>
@@ -6567,10 +6567,10 @@
         <v>MM020070</v>
       </c>
       <c r="C163">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D163">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E163">
         <v>20</v>
@@ -6601,10 +6601,10 @@
         <v>MM030070</v>
       </c>
       <c r="C164">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D164">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E164">
         <v>30</v>
@@ -6635,10 +6635,10 @@
         <v>MM040070</v>
       </c>
       <c r="C165">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D165">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E165">
         <v>40</v>
@@ -6669,10 +6669,10 @@
         <v>MM050070</v>
       </c>
       <c r="C166">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D166">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E166">
         <v>50</v>
@@ -6703,10 +6703,10 @@
         <v>MM060070</v>
       </c>
       <c r="C167">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D167">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E167">
         <v>60</v>
@@ -6737,10 +6737,10 @@
         <v>MM070070</v>
       </c>
       <c r="C168">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D168">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E168">
         <v>70</v>
@@ -6771,10 +6771,10 @@
         <v>MM080070</v>
       </c>
       <c r="C169">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D169">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E169">
         <v>80</v>
@@ -6805,10 +6805,10 @@
         <v>MM090070</v>
       </c>
       <c r="C170">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D170">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E170">
         <v>90</v>
@@ -6839,10 +6839,10 @@
         <v>MM100070</v>
       </c>
       <c r="C171">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D171">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E171">
         <v>100</v>
@@ -6873,10 +6873,10 @@
         <v>MM010080</v>
       </c>
       <c r="C172">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D172">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E172">
         <v>10</v>
@@ -6907,10 +6907,10 @@
         <v>MM020080</v>
       </c>
       <c r="C173">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D173">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E173">
         <v>20</v>
@@ -6941,10 +6941,10 @@
         <v>MM030080</v>
       </c>
       <c r="C174">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D174">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E174">
         <v>30</v>
@@ -6975,10 +6975,10 @@
         <v>MM040080</v>
       </c>
       <c r="C175">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D175">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E175">
         <v>40</v>
@@ -7009,10 +7009,10 @@
         <v>MM050080</v>
       </c>
       <c r="C176">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D176">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E176">
         <v>50</v>
@@ -7043,10 +7043,10 @@
         <v>MM060080</v>
       </c>
       <c r="C177">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D177">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E177">
         <v>60</v>
@@ -7077,10 +7077,10 @@
         <v>MM070080</v>
       </c>
       <c r="C178">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D178">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E178">
         <v>70</v>
@@ -7111,10 +7111,10 @@
         <v>MM080080</v>
       </c>
       <c r="C179">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D179">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E179">
         <v>80</v>
@@ -7145,10 +7145,10 @@
         <v>MM090080</v>
       </c>
       <c r="C180">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D180">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E180">
         <v>90</v>
@@ -7179,10 +7179,10 @@
         <v>MM100080</v>
       </c>
       <c r="C181">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D181">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E181">
         <v>100</v>
@@ -7213,10 +7213,10 @@
         <v>MM010090</v>
       </c>
       <c r="C182">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D182">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E182">
         <v>10</v>
@@ -7247,10 +7247,10 @@
         <v>MM020090</v>
       </c>
       <c r="C183">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D183">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E183">
         <v>20</v>
@@ -7281,10 +7281,10 @@
         <v>MM030090</v>
       </c>
       <c r="C184">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D184">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E184">
         <v>30</v>
@@ -7315,10 +7315,10 @@
         <v>MM040090</v>
       </c>
       <c r="C185">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D185">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E185">
         <v>40</v>
@@ -7349,10 +7349,10 @@
         <v>MM050090</v>
       </c>
       <c r="C186">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D186">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E186">
         <v>50</v>
@@ -7383,10 +7383,10 @@
         <v>MM060090</v>
       </c>
       <c r="C187">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D187">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E187">
         <v>60</v>
@@ -7417,10 +7417,10 @@
         <v>MM070090</v>
       </c>
       <c r="C188">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D188">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E188">
         <v>70</v>
@@ -7451,10 +7451,10 @@
         <v>MM080090</v>
       </c>
       <c r="C189">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D189">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E189">
         <v>80</v>
@@ -7485,10 +7485,10 @@
         <v>MM090090</v>
       </c>
       <c r="C190">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D190">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E190">
         <v>90</v>
@@ -7519,10 +7519,10 @@
         <v>MM100090</v>
       </c>
       <c r="C191">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D191">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E191">
         <v>100</v>
@@ -7553,10 +7553,10 @@
         <v>MM010100</v>
       </c>
       <c r="C192">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D192">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E192">
         <v>10</v>
@@ -7587,10 +7587,10 @@
         <v>MM020100</v>
       </c>
       <c r="C193">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D193">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E193">
         <v>20</v>
@@ -7621,10 +7621,10 @@
         <v>MM030100</v>
       </c>
       <c r="C194">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D194">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E194">
         <v>30</v>
@@ -7655,10 +7655,10 @@
         <v>MM040100</v>
       </c>
       <c r="C195">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D195">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E195">
         <v>40</v>
@@ -7689,10 +7689,10 @@
         <v>MM050100</v>
       </c>
       <c r="C196">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D196">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E196">
         <v>50</v>
@@ -7723,10 +7723,10 @@
         <v>MM060100</v>
       </c>
       <c r="C197">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D197">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E197">
         <v>60</v>
@@ -7757,10 +7757,10 @@
         <v>MM070100</v>
       </c>
       <c r="C198">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D198">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E198">
         <v>70</v>
@@ -7791,10 +7791,10 @@
         <v>MM080100</v>
       </c>
       <c r="C199">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D199">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E199">
         <v>80</v>
@@ -7825,10 +7825,10 @@
         <v>MM090100</v>
       </c>
       <c r="C200">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D200">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E200">
         <v>90</v>
@@ -7859,10 +7859,10 @@
         <v>MM100100</v>
       </c>
       <c r="C201">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D201">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E201">
         <v>100</v>
@@ -8241,7 +8241,7 @@
         <v>44768</v>
       </c>
       <c r="B212" t="str">
-        <f t="shared" ref="B212:B222" si="10">I212&amp;TEXT(E212,"000")&amp;TEXT(F212,"000")</f>
+        <f t="shared" ref="B212:B221" si="10">I212&amp;TEXT(E212,"000")&amp;TEXT(F212,"000")</f>
         <v>MM000000</v>
       </c>
       <c r="C212">

</xml_diff>

<commit_message>
V = n_V_[T] fixed
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/65e5ba34f41e25e0/lab/aespa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1010" documentId="13_ncr:40009_{B2571C16-CD38-4085-A61D-8240FBC2AD0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05E49A54-B606-4806-B13C-EBDE44318F39}"/>
+  <xr:revisionPtr revIDLastSave="1022" documentId="13_ncr:40009_{B2571C16-CD38-4085-A61D-8240FBC2AD0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E35C88E-8CEE-40B8-9094-FBB629CB72CC}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="3360" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1057,8 +1057,8 @@
   <dimension ref="A1:K226"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I76" sqref="I76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
@@ -1110,10 +1110,10 @@
         <v>MM010010</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D2">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E2">
         <v>10</v>
@@ -1143,10 +1143,10 @@
         <v>MM020010</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D3">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E3">
         <v>20</v>
@@ -1176,10 +1176,10 @@
         <v>MM030010</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D4">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E4">
         <v>30</v>
@@ -1209,10 +1209,10 @@
         <v>MM040010</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D5">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E5">
         <v>40</v>
@@ -1242,10 +1242,10 @@
         <v>MM050010</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D6">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E6">
         <v>50</v>
@@ -1275,10 +1275,10 @@
         <v>MM060010</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D7">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E7">
         <v>60</v>
@@ -1308,10 +1308,10 @@
         <v>MM070010</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D8">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E8">
         <v>70</v>
@@ -1341,10 +1341,10 @@
         <v>MM080010</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D9">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E9">
         <v>80</v>
@@ -1374,10 +1374,10 @@
         <v>MM090010</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D10">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E10">
         <v>90</v>
@@ -1407,10 +1407,10 @@
         <v>MM100010</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D11">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E11">
         <v>100</v>
@@ -1440,10 +1440,10 @@
         <v>MM010020</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D12">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E12">
         <v>10</v>
@@ -1474,10 +1474,10 @@
         <v>MM020020</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D13">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E13">
         <v>20</v>
@@ -1508,10 +1508,10 @@
         <v>MM030020</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D14">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E14">
         <v>30</v>
@@ -1542,10 +1542,10 @@
         <v>MM040020</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D15">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E15">
         <v>40</v>
@@ -1576,10 +1576,10 @@
         <v>MM050020</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D16">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E16">
         <v>50</v>
@@ -1610,10 +1610,10 @@
         <v>MM060020</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D17">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E17">
         <v>60</v>
@@ -1644,10 +1644,10 @@
         <v>MM070020</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D18">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E18">
         <v>70</v>
@@ -1678,10 +1678,10 @@
         <v>MM080020</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D19">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E19">
         <v>80</v>
@@ -1712,10 +1712,10 @@
         <v>MM090020</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D20">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E20">
         <v>90</v>
@@ -1746,10 +1746,10 @@
         <v>MM100020</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D21">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E21">
         <v>100</v>
@@ -1780,10 +1780,10 @@
         <v>MM010030</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D22">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E22">
         <v>10</v>
@@ -1814,10 +1814,10 @@
         <v>MM020030</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D23">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E23">
         <v>20</v>
@@ -1848,10 +1848,10 @@
         <v>MM030030</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D24">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E24">
         <v>30</v>
@@ -1882,10 +1882,10 @@
         <v>MM040030</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D25">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E25">
         <v>40</v>
@@ -1916,10 +1916,10 @@
         <v>MM050030</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D26">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E26">
         <v>50</v>
@@ -1950,10 +1950,10 @@
         <v>MM060030</v>
       </c>
       <c r="C27">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D27">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E27">
         <v>60</v>
@@ -1984,10 +1984,10 @@
         <v>MM070030</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D28">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E28">
         <v>70</v>
@@ -2018,10 +2018,10 @@
         <v>MM080030</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D29">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E29">
         <v>80</v>
@@ -2052,10 +2052,10 @@
         <v>MM090030</v>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D30">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E30">
         <v>90</v>
@@ -2086,10 +2086,10 @@
         <v>MM100030</v>
       </c>
       <c r="C31">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D31">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E31">
         <v>100</v>
@@ -2120,10 +2120,10 @@
         <v>MM010040</v>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D32">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E32">
         <v>10</v>
@@ -2154,10 +2154,10 @@
         <v>MM020040</v>
       </c>
       <c r="C33">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D33">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E33">
         <v>20</v>
@@ -2188,10 +2188,10 @@
         <v>MM030040</v>
       </c>
       <c r="C34">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D34">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E34">
         <v>30</v>
@@ -2222,10 +2222,10 @@
         <v>MM040040</v>
       </c>
       <c r="C35">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D35">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E35">
         <v>40</v>
@@ -2256,10 +2256,10 @@
         <v>MM050040</v>
       </c>
       <c r="C36">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D36">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E36">
         <v>50</v>
@@ -2290,10 +2290,10 @@
         <v>MM060040</v>
       </c>
       <c r="C37">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D37">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E37">
         <v>60</v>
@@ -2324,10 +2324,10 @@
         <v>MM070040</v>
       </c>
       <c r="C38">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D38">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E38">
         <v>70</v>
@@ -2358,10 +2358,10 @@
         <v>MM080040</v>
       </c>
       <c r="C39">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D39">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E39">
         <v>80</v>
@@ -2392,10 +2392,10 @@
         <v>MM090040</v>
       </c>
       <c r="C40">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D40">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E40">
         <v>90</v>
@@ -2426,10 +2426,10 @@
         <v>MM100040</v>
       </c>
       <c r="C41">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D41">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E41">
         <v>100</v>
@@ -2460,10 +2460,10 @@
         <v>MM010050</v>
       </c>
       <c r="C42">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D42">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E42">
         <v>10</v>
@@ -2494,10 +2494,10 @@
         <v>MM020050</v>
       </c>
       <c r="C43">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D43">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E43">
         <v>20</v>
@@ -2528,10 +2528,10 @@
         <v>MM030050</v>
       </c>
       <c r="C44">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D44">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E44">
         <v>30</v>
@@ -2562,10 +2562,10 @@
         <v>MM040050</v>
       </c>
       <c r="C45">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D45">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E45">
         <v>40</v>
@@ -2596,10 +2596,10 @@
         <v>MM050050</v>
       </c>
       <c r="C46">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D46">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E46">
         <v>50</v>
@@ -2630,10 +2630,10 @@
         <v>MM060050</v>
       </c>
       <c r="C47">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D47">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E47">
         <v>60</v>
@@ -2664,10 +2664,10 @@
         <v>MM070050</v>
       </c>
       <c r="C48">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D48">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E48">
         <v>70</v>
@@ -2698,10 +2698,10 @@
         <v>MM080050</v>
       </c>
       <c r="C49">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D49">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E49">
         <v>80</v>
@@ -2732,10 +2732,10 @@
         <v>MM090050</v>
       </c>
       <c r="C50">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D50">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E50">
         <v>90</v>
@@ -2766,10 +2766,10 @@
         <v>MM100050</v>
       </c>
       <c r="C51">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D51">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E51">
         <v>100</v>
@@ -2800,10 +2800,10 @@
         <v>MM010060</v>
       </c>
       <c r="C52">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D52">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E52">
         <v>10</v>
@@ -2834,10 +2834,10 @@
         <v>MM020060</v>
       </c>
       <c r="C53">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D53">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E53">
         <v>20</v>
@@ -2868,10 +2868,10 @@
         <v>MM030060</v>
       </c>
       <c r="C54">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D54">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E54">
         <v>30</v>
@@ -2902,10 +2902,10 @@
         <v>MM040060</v>
       </c>
       <c r="C55">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D55">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E55">
         <v>40</v>
@@ -2936,10 +2936,10 @@
         <v>MM050060</v>
       </c>
       <c r="C56">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D56">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E56">
         <v>50</v>
@@ -2970,10 +2970,10 @@
         <v>MM060060</v>
       </c>
       <c r="C57">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D57">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E57">
         <v>60</v>
@@ -3004,10 +3004,10 @@
         <v>MM070060</v>
       </c>
       <c r="C58">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D58">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E58">
         <v>70</v>
@@ -3038,10 +3038,10 @@
         <v>MM080060</v>
       </c>
       <c r="C59">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D59">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E59">
         <v>80</v>
@@ -3072,10 +3072,10 @@
         <v>MM090060</v>
       </c>
       <c r="C60">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D60">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E60">
         <v>90</v>
@@ -3106,10 +3106,10 @@
         <v>MM100060</v>
       </c>
       <c r="C61">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D61">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E61">
         <v>100</v>
@@ -3140,10 +3140,10 @@
         <v>MM010070</v>
       </c>
       <c r="C62">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D62">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E62">
         <v>10</v>
@@ -3174,10 +3174,10 @@
         <v>MM020070</v>
       </c>
       <c r="C63">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D63">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E63">
         <v>20</v>
@@ -3208,10 +3208,10 @@
         <v>MM030070</v>
       </c>
       <c r="C64">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D64">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E64">
         <v>30</v>
@@ -3242,10 +3242,10 @@
         <v>MM040070</v>
       </c>
       <c r="C65">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D65">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E65">
         <v>40</v>
@@ -3276,10 +3276,10 @@
         <v>MM050070</v>
       </c>
       <c r="C66">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D66">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E66">
         <v>50</v>
@@ -3310,10 +3310,10 @@
         <v>MM060070</v>
       </c>
       <c r="C67">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D67">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E67">
         <v>60</v>
@@ -3344,10 +3344,10 @@
         <v>MM070070</v>
       </c>
       <c r="C68">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D68">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E68">
         <v>70</v>
@@ -3378,10 +3378,10 @@
         <v>MM080070</v>
       </c>
       <c r="C69">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D69">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E69">
         <v>80</v>
@@ -3412,10 +3412,10 @@
         <v>MM090070</v>
       </c>
       <c r="C70">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D70">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E70">
         <v>90</v>
@@ -3446,10 +3446,10 @@
         <v>MM100070</v>
       </c>
       <c r="C71">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D71">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E71">
         <v>100</v>
@@ -3480,10 +3480,10 @@
         <v>MM010080</v>
       </c>
       <c r="C72">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D72">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E72">
         <v>10</v>
@@ -3514,10 +3514,10 @@
         <v>MM020080</v>
       </c>
       <c r="C73">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D73">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E73">
         <v>20</v>
@@ -3548,10 +3548,10 @@
         <v>MM030080</v>
       </c>
       <c r="C74">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D74">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E74">
         <v>30</v>
@@ -3582,10 +3582,10 @@
         <v>MM040080</v>
       </c>
       <c r="C75">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D75">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E75">
         <v>40</v>
@@ -3616,10 +3616,10 @@
         <v>MM050080</v>
       </c>
       <c r="C76">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D76">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E76">
         <v>50</v>
@@ -3650,10 +3650,10 @@
         <v>MM060080</v>
       </c>
       <c r="C77">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D77">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E77">
         <v>60</v>
@@ -3684,10 +3684,10 @@
         <v>MM070080</v>
       </c>
       <c r="C78">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D78">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E78">
         <v>70</v>
@@ -3718,10 +3718,10 @@
         <v>MM080080</v>
       </c>
       <c r="C79">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D79">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E79">
         <v>80</v>
@@ -3752,10 +3752,10 @@
         <v>MM090080</v>
       </c>
       <c r="C80">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D80">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E80">
         <v>90</v>
@@ -3786,10 +3786,10 @@
         <v>MM100080</v>
       </c>
       <c r="C81">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D81">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E81">
         <v>100</v>
@@ -3820,10 +3820,10 @@
         <v>MM010090</v>
       </c>
       <c r="C82">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D82">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E82">
         <v>10</v>
@@ -3854,10 +3854,10 @@
         <v>MM020090</v>
       </c>
       <c r="C83">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D83">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E83">
         <v>20</v>
@@ -3888,10 +3888,10 @@
         <v>MM030090</v>
       </c>
       <c r="C84">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D84">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E84">
         <v>30</v>
@@ -3922,10 +3922,10 @@
         <v>MM040090</v>
       </c>
       <c r="C85">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D85">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E85">
         <v>40</v>
@@ -3956,10 +3956,10 @@
         <v>MM050090</v>
       </c>
       <c r="C86">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D86">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E86">
         <v>50</v>
@@ -3990,10 +3990,10 @@
         <v>MM060090</v>
       </c>
       <c r="C87">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D87">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E87">
         <v>60</v>
@@ -4024,10 +4024,10 @@
         <v>MM070090</v>
       </c>
       <c r="C88">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D88">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E88">
         <v>70</v>
@@ -4058,10 +4058,10 @@
         <v>MM080090</v>
       </c>
       <c r="C89">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D89">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E89">
         <v>80</v>
@@ -4092,10 +4092,10 @@
         <v>MM090090</v>
       </c>
       <c r="C90">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D90">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E90">
         <v>90</v>
@@ -4126,10 +4126,10 @@
         <v>MM100090</v>
       </c>
       <c r="C91">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D91">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E91">
         <v>100</v>
@@ -4160,10 +4160,10 @@
         <v>MM010100</v>
       </c>
       <c r="C92">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D92">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E92">
         <v>10</v>
@@ -4194,10 +4194,10 @@
         <v>MM020100</v>
       </c>
       <c r="C93">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D93">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E93">
         <v>20</v>
@@ -4228,10 +4228,10 @@
         <v>MM030100</v>
       </c>
       <c r="C94">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D94">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E94">
         <v>30</v>
@@ -4262,10 +4262,10 @@
         <v>MM040100</v>
       </c>
       <c r="C95">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D95">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E95">
         <v>40</v>
@@ -4296,10 +4296,10 @@
         <v>MM050100</v>
       </c>
       <c r="C96">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D96">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E96">
         <v>50</v>
@@ -4330,10 +4330,10 @@
         <v>MM060100</v>
       </c>
       <c r="C97">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D97">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E97">
         <v>60</v>
@@ -4364,10 +4364,10 @@
         <v>MM070100</v>
       </c>
       <c r="C98">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D98">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E98">
         <v>70</v>
@@ -4398,10 +4398,10 @@
         <v>MM080100</v>
       </c>
       <c r="C99">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D99">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E99">
         <v>80</v>
@@ -4432,10 +4432,10 @@
         <v>MM090100</v>
       </c>
       <c r="C100">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D100">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E100">
         <v>90</v>
@@ -4466,10 +4466,10 @@
         <v>MM100100</v>
       </c>
       <c r="C101">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D101">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E101">
         <v>100</v>
@@ -4503,10 +4503,10 @@
         <v>MM010010</v>
       </c>
       <c r="C102">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D102">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E102">
         <v>10</v>
@@ -4536,10 +4536,10 @@
         <v>MM020010</v>
       </c>
       <c r="C103">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D103">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E103">
         <v>20</v>
@@ -4569,10 +4569,10 @@
         <v>MM030010</v>
       </c>
       <c r="C104">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D104">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E104">
         <v>30</v>
@@ -4602,10 +4602,10 @@
         <v>MM040010</v>
       </c>
       <c r="C105">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D105">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E105">
         <v>40</v>
@@ -4635,10 +4635,10 @@
         <v>MM050010</v>
       </c>
       <c r="C106">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D106">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E106">
         <v>50</v>
@@ -4668,10 +4668,10 @@
         <v>MM060010</v>
       </c>
       <c r="C107">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D107">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E107">
         <v>60</v>
@@ -4701,10 +4701,10 @@
         <v>MM070010</v>
       </c>
       <c r="C108">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D108">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E108">
         <v>70</v>
@@ -4734,10 +4734,10 @@
         <v>MM080010</v>
       </c>
       <c r="C109">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D109">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E109">
         <v>80</v>
@@ -4767,10 +4767,10 @@
         <v>MM090010</v>
       </c>
       <c r="C110">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D110">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E110">
         <v>90</v>
@@ -4800,10 +4800,10 @@
         <v>MM100010</v>
       </c>
       <c r="C111">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D111">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E111">
         <v>100</v>
@@ -4833,10 +4833,10 @@
         <v>MM010020</v>
       </c>
       <c r="C112">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D112">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E112">
         <v>10</v>
@@ -4867,10 +4867,10 @@
         <v>MM020020</v>
       </c>
       <c r="C113">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D113">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E113">
         <v>20</v>
@@ -4901,10 +4901,10 @@
         <v>MM030020</v>
       </c>
       <c r="C114">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D114">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E114">
         <v>30</v>
@@ -4935,10 +4935,10 @@
         <v>MM040020</v>
       </c>
       <c r="C115">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D115">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E115">
         <v>40</v>
@@ -4969,10 +4969,10 @@
         <v>MM050020</v>
       </c>
       <c r="C116">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D116">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E116">
         <v>50</v>
@@ -5003,10 +5003,10 @@
         <v>MM060020</v>
       </c>
       <c r="C117">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D117">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E117">
         <v>60</v>
@@ -5037,10 +5037,10 @@
         <v>MM070020</v>
       </c>
       <c r="C118">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D118">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E118">
         <v>70</v>
@@ -5071,10 +5071,10 @@
         <v>MM080020</v>
       </c>
       <c r="C119">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D119">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E119">
         <v>80</v>
@@ -5105,10 +5105,10 @@
         <v>MM090020</v>
       </c>
       <c r="C120">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D120">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E120">
         <v>90</v>
@@ -5139,10 +5139,10 @@
         <v>MM100020</v>
       </c>
       <c r="C121">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D121">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E121">
         <v>100</v>
@@ -5173,10 +5173,10 @@
         <v>MM010030</v>
       </c>
       <c r="C122">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D122">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E122">
         <v>10</v>
@@ -5207,10 +5207,10 @@
         <v>MM020030</v>
       </c>
       <c r="C123">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D123">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E123">
         <v>20</v>
@@ -5241,10 +5241,10 @@
         <v>MM030030</v>
       </c>
       <c r="C124">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D124">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E124">
         <v>30</v>
@@ -5275,10 +5275,10 @@
         <v>MM040030</v>
       </c>
       <c r="C125">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D125">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E125">
         <v>40</v>
@@ -5309,10 +5309,10 @@
         <v>MM050030</v>
       </c>
       <c r="C126">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D126">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E126">
         <v>50</v>
@@ -5343,10 +5343,10 @@
         <v>MM060030</v>
       </c>
       <c r="C127">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D127">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E127">
         <v>60</v>
@@ -5377,10 +5377,10 @@
         <v>MM070030</v>
       </c>
       <c r="C128">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D128">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E128">
         <v>70</v>
@@ -5411,10 +5411,10 @@
         <v>MM080030</v>
       </c>
       <c r="C129">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D129">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E129">
         <v>80</v>
@@ -5445,10 +5445,10 @@
         <v>MM090030</v>
       </c>
       <c r="C130">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D130">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E130">
         <v>90</v>
@@ -5479,10 +5479,10 @@
         <v>MM100030</v>
       </c>
       <c r="C131">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D131">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E131">
         <v>100</v>
@@ -5513,10 +5513,10 @@
         <v>MM010040</v>
       </c>
       <c r="C132">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D132">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E132">
         <v>10</v>
@@ -5547,10 +5547,10 @@
         <v>MM020040</v>
       </c>
       <c r="C133">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D133">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E133">
         <v>20</v>
@@ -5581,10 +5581,10 @@
         <v>MM030040</v>
       </c>
       <c r="C134">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D134">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E134">
         <v>30</v>
@@ -5615,10 +5615,10 @@
         <v>MM040040</v>
       </c>
       <c r="C135">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D135">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E135">
         <v>40</v>
@@ -5649,10 +5649,10 @@
         <v>MM050040</v>
       </c>
       <c r="C136">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D136">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E136">
         <v>50</v>
@@ -5683,10 +5683,10 @@
         <v>MM060040</v>
       </c>
       <c r="C137">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D137">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E137">
         <v>60</v>
@@ -5717,10 +5717,10 @@
         <v>MM070040</v>
       </c>
       <c r="C138">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D138">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E138">
         <v>70</v>
@@ -5751,10 +5751,10 @@
         <v>MM080040</v>
       </c>
       <c r="C139">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D139">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E139">
         <v>80</v>
@@ -5785,10 +5785,10 @@
         <v>MM090040</v>
       </c>
       <c r="C140">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D140">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E140">
         <v>90</v>
@@ -5819,10 +5819,10 @@
         <v>MM100040</v>
       </c>
       <c r="C141">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D141">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E141">
         <v>100</v>
@@ -5853,10 +5853,10 @@
         <v>MM010050</v>
       </c>
       <c r="C142">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D142">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E142">
         <v>10</v>
@@ -5887,10 +5887,10 @@
         <v>MM020050</v>
       </c>
       <c r="C143">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D143">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E143">
         <v>20</v>
@@ -5921,10 +5921,10 @@
         <v>MM030050</v>
       </c>
       <c r="C144">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D144">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E144">
         <v>30</v>
@@ -5955,10 +5955,10 @@
         <v>MM040050</v>
       </c>
       <c r="C145">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D145">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E145">
         <v>40</v>
@@ -5989,10 +5989,10 @@
         <v>MM050050</v>
       </c>
       <c r="C146">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D146">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E146">
         <v>50</v>
@@ -6023,10 +6023,10 @@
         <v>MM060050</v>
       </c>
       <c r="C147">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D147">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E147">
         <v>60</v>
@@ -6057,10 +6057,10 @@
         <v>MM070050</v>
       </c>
       <c r="C148">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D148">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E148">
         <v>70</v>
@@ -6091,10 +6091,10 @@
         <v>MM080050</v>
       </c>
       <c r="C149">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D149">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E149">
         <v>80</v>
@@ -6125,10 +6125,10 @@
         <v>MM090050</v>
       </c>
       <c r="C150">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D150">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E150">
         <v>90</v>
@@ -6159,10 +6159,10 @@
         <v>MM100050</v>
       </c>
       <c r="C151">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D151">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E151">
         <v>100</v>
@@ -6193,10 +6193,10 @@
         <v>MM010060</v>
       </c>
       <c r="C152">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D152">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E152">
         <v>10</v>
@@ -6227,10 +6227,10 @@
         <v>MM020060</v>
       </c>
       <c r="C153">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D153">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E153">
         <v>20</v>
@@ -6261,10 +6261,10 @@
         <v>MM030060</v>
       </c>
       <c r="C154">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D154">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E154">
         <v>30</v>
@@ -6295,10 +6295,10 @@
         <v>MM040060</v>
       </c>
       <c r="C155">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D155">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E155">
         <v>40</v>
@@ -6329,10 +6329,10 @@
         <v>MM050060</v>
       </c>
       <c r="C156">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D156">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E156">
         <v>50</v>
@@ -6363,10 +6363,10 @@
         <v>MM060060</v>
       </c>
       <c r="C157">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D157">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E157">
         <v>60</v>
@@ -6397,10 +6397,10 @@
         <v>MM070060</v>
       </c>
       <c r="C158">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D158">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E158">
         <v>70</v>
@@ -6431,10 +6431,10 @@
         <v>MM080060</v>
       </c>
       <c r="C159">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D159">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E159">
         <v>80</v>
@@ -6465,10 +6465,10 @@
         <v>MM090060</v>
       </c>
       <c r="C160">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D160">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E160">
         <v>90</v>
@@ -6499,10 +6499,10 @@
         <v>MM100060</v>
       </c>
       <c r="C161">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D161">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E161">
         <v>100</v>
@@ -6533,10 +6533,10 @@
         <v>MM010070</v>
       </c>
       <c r="C162">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D162">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E162">
         <v>10</v>
@@ -6567,10 +6567,10 @@
         <v>MM020070</v>
       </c>
       <c r="C163">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D163">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E163">
         <v>20</v>
@@ -6601,10 +6601,10 @@
         <v>MM030070</v>
       </c>
       <c r="C164">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D164">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E164">
         <v>30</v>
@@ -6635,10 +6635,10 @@
         <v>MM040070</v>
       </c>
       <c r="C165">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D165">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E165">
         <v>40</v>
@@ -6669,10 +6669,10 @@
         <v>MM050070</v>
       </c>
       <c r="C166">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D166">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E166">
         <v>50</v>
@@ -6703,10 +6703,10 @@
         <v>MM060070</v>
       </c>
       <c r="C167">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D167">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E167">
         <v>60</v>
@@ -6737,10 +6737,10 @@
         <v>MM070070</v>
       </c>
       <c r="C168">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D168">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E168">
         <v>70</v>
@@ -6771,10 +6771,10 @@
         <v>MM080070</v>
       </c>
       <c r="C169">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D169">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E169">
         <v>80</v>
@@ -6805,10 +6805,10 @@
         <v>MM090070</v>
       </c>
       <c r="C170">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D170">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E170">
         <v>90</v>
@@ -6839,10 +6839,10 @@
         <v>MM100070</v>
       </c>
       <c r="C171">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D171">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E171">
         <v>100</v>
@@ -6873,10 +6873,10 @@
         <v>MM010080</v>
       </c>
       <c r="C172">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D172">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E172">
         <v>10</v>
@@ -6907,10 +6907,10 @@
         <v>MM020080</v>
       </c>
       <c r="C173">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D173">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E173">
         <v>20</v>
@@ -6941,10 +6941,10 @@
         <v>MM030080</v>
       </c>
       <c r="C174">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D174">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E174">
         <v>30</v>
@@ -6975,10 +6975,10 @@
         <v>MM040080</v>
       </c>
       <c r="C175">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D175">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E175">
         <v>40</v>
@@ -7009,10 +7009,10 @@
         <v>MM050080</v>
       </c>
       <c r="C176">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D176">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E176">
         <v>50</v>
@@ -7043,10 +7043,10 @@
         <v>MM060080</v>
       </c>
       <c r="C177">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D177">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E177">
         <v>60</v>
@@ -7077,10 +7077,10 @@
         <v>MM070080</v>
       </c>
       <c r="C178">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D178">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E178">
         <v>70</v>
@@ -7111,10 +7111,10 @@
         <v>MM080080</v>
       </c>
       <c r="C179">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D179">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E179">
         <v>80</v>
@@ -7145,10 +7145,10 @@
         <v>MM090080</v>
       </c>
       <c r="C180">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D180">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E180">
         <v>90</v>
@@ -7179,10 +7179,10 @@
         <v>MM100080</v>
       </c>
       <c r="C181">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D181">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E181">
         <v>100</v>
@@ -7213,10 +7213,10 @@
         <v>MM010090</v>
       </c>
       <c r="C182">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D182">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E182">
         <v>10</v>
@@ -7247,10 +7247,10 @@
         <v>MM020090</v>
       </c>
       <c r="C183">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D183">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E183">
         <v>20</v>
@@ -7281,10 +7281,10 @@
         <v>MM030090</v>
       </c>
       <c r="C184">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D184">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E184">
         <v>30</v>
@@ -7315,10 +7315,10 @@
         <v>MM040090</v>
       </c>
       <c r="C185">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D185">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E185">
         <v>40</v>
@@ -7349,10 +7349,10 @@
         <v>MM050090</v>
       </c>
       <c r="C186">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D186">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E186">
         <v>50</v>
@@ -7383,10 +7383,10 @@
         <v>MM060090</v>
       </c>
       <c r="C187">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D187">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E187">
         <v>60</v>
@@ -7417,10 +7417,10 @@
         <v>MM070090</v>
       </c>
       <c r="C188">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D188">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E188">
         <v>70</v>
@@ -7451,10 +7451,10 @@
         <v>MM080090</v>
       </c>
       <c r="C189">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D189">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E189">
         <v>80</v>
@@ -7485,10 +7485,10 @@
         <v>MM090090</v>
       </c>
       <c r="C190">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D190">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E190">
         <v>90</v>
@@ -7519,10 +7519,10 @@
         <v>MM100090</v>
       </c>
       <c r="C191">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D191">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E191">
         <v>100</v>
@@ -7553,10 +7553,10 @@
         <v>MM010100</v>
       </c>
       <c r="C192">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D192">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E192">
         <v>10</v>
@@ -7587,10 +7587,10 @@
         <v>MM020100</v>
       </c>
       <c r="C193">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D193">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E193">
         <v>20</v>
@@ -7621,10 +7621,10 @@
         <v>MM030100</v>
       </c>
       <c r="C194">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D194">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E194">
         <v>30</v>
@@ -7655,10 +7655,10 @@
         <v>MM040100</v>
       </c>
       <c r="C195">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D195">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E195">
         <v>40</v>
@@ -7689,10 +7689,10 @@
         <v>MM050100</v>
       </c>
       <c r="C196">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D196">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E196">
         <v>50</v>
@@ -7723,10 +7723,10 @@
         <v>MM060100</v>
       </c>
       <c r="C197">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D197">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E197">
         <v>60</v>
@@ -7757,10 +7757,10 @@
         <v>MM070100</v>
       </c>
       <c r="C198">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D198">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E198">
         <v>70</v>
@@ -7791,10 +7791,10 @@
         <v>MM080100</v>
       </c>
       <c r="C199">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D199">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E199">
         <v>80</v>
@@ -7825,10 +7825,10 @@
         <v>MM090100</v>
       </c>
       <c r="C200">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D200">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E200">
         <v>90</v>
@@ -7859,10 +7859,10 @@
         <v>MM100100</v>
       </c>
       <c r="C201">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D201">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E201">
         <v>100</v>

</xml_diff>